<commit_message>
Updated Model for Coding
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drewd\Documents\repos\satcomm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{394EEDD9-7E5D-48A6-AFFC-BAE692149EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BACC4CC-D4F4-4568-8605-94F9F8830341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0A52E5C-8B66-4095-BE98-79E918536ADA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>LNA 1</t>
   </si>
@@ -169,6 +169,27 @@
   </si>
   <si>
     <t>1.6 dB IL, 45 dB Rejection</t>
+  </si>
+  <si>
+    <t>BandPassFilterKa</t>
+  </si>
+  <si>
+    <t>1.3dB IL</t>
+  </si>
+  <si>
+    <t>https://www.minicircuits.com/WebStore/dashboard.html?model=ZVBP-40600-K%2B</t>
+  </si>
+  <si>
+    <t>HPA KA</t>
+  </si>
+  <si>
+    <t>https://rfessentials.com/full-ka-band-high-power-amplifier-26-ghz-to-40-ghz/</t>
+  </si>
+  <si>
+    <t>Mixer</t>
+  </si>
+  <si>
+    <t>https://www.qorvo.com/products/p/CMD313</t>
   </si>
 </sst>
 </file>
@@ -531,14 +552,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8D4279-B10E-4006-884E-6151387C624F}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="98.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
@@ -748,14 +770,56 @@
         <v>44</v>
       </c>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26">
+        <v>35</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>-8</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" tooltip="https://www.ums-rf.com/wp-content/uploads/2017/01/CHA1077a98F-Full-8266.pdf" xr:uid="{552CA2C7-45F3-4032-99DC-FA0564170F1B}"/>
     <hyperlink ref="F15" r:id="rId2" xr:uid="{B74758A4-30EC-482A-8D40-5FE4567ACF4A}"/>
     <hyperlink ref="E18" r:id="rId3" xr:uid="{3836D737-E77C-4DA1-B496-ABE5B447AADE}"/>
     <hyperlink ref="E21" r:id="rId4" xr:uid="{4A2CE6E6-C434-4AAA-B958-22726CEDC911}"/>
+    <hyperlink ref="E24" r:id="rId5" xr:uid="{594B1AA5-9199-4168-82CE-8E1B9064CDE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>